<commit_message>
further works on data import
</commit_message>
<xml_diff>
--- a/lib-data.xlsx
+++ b/lib-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaszeluk\Documents\projekty\melvil-inkubator\melvil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE5AA70-41B3-498B-BE3D-41D42C456DC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025E4D26-CC37-4B17-891A-93951D5D710A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="715">
   <si>
     <t>Lp.</t>
   </si>
@@ -2103,6 +2103,78 @@
   </si>
   <si>
     <t>Forbes raport specjalny 10/2011 Kto jest kim w polskiej bankowości 2011</t>
+  </si>
+  <si>
+    <t>numer</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>12-1</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48/880</t>
   </si>
 </sst>
 </file>
@@ -2298,7 +2370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2442,6 +2514,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -24549,8 +24627,8 @@
   </sheetPr>
   <dimension ref="A1:H997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G41" activeCellId="3" sqref="D1:D1048576 E1:E1048576 F1:F1048576 G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24573,1044 +24651,1230 @@
       <c r="C1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="39"/>
+      <c r="D1" s="63" t="s">
+        <v>691</v>
+      </c>
       <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:8" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64"/>
+      <c r="A2" s="66"/>
       <c r="B2" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="60">
         <v>2010</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="64">
+        <v>0</v>
+      </c>
       <c r="E2" s="56"/>
       <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:8" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="64"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="60">
         <v>2011</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="64">
+        <v>13</v>
+      </c>
       <c r="E3" s="56"/>
       <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="64">
+        <v>39</v>
+      </c>
       <c r="E4" s="56"/>
       <c r="H4" s="58"/>
     </row>
     <row r="5" spans="1:8" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="64"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="64">
+        <v>17</v>
+      </c>
       <c r="E5" s="56"/>
       <c r="H5" s="58"/>
     </row>
     <row r="6" spans="1:8" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="64"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="64">
+        <v>1</v>
+      </c>
       <c r="E6" s="56"/>
       <c r="H6" s="58"/>
     </row>
     <row r="7" spans="1:8" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="64"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="64">
+        <v>9</v>
+      </c>
       <c r="E7" s="56"/>
       <c r="H7" s="58"/>
     </row>
     <row r="8" spans="1:8" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="64"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="56"/>
+      <c r="D8" s="64">
+        <v>21</v>
+      </c>
       <c r="E8" s="56"/>
       <c r="H8" s="58"/>
     </row>
     <row r="9" spans="1:8" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="64"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="56" t="s">
         <v>689</v>
       </c>
       <c r="C9" s="59">
         <v>2016</v>
       </c>
-      <c r="D9" s="56"/>
+      <c r="D9" s="64">
+        <v>2</v>
+      </c>
       <c r="E9" s="56"/>
       <c r="F9" s="61"/>
       <c r="H9" s="58"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="63">
+        <v>5</v>
+      </c>
       <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="63">
+        <v>6</v>
+      </c>
       <c r="E11" s="39"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="63">
+        <v>7</v>
+      </c>
       <c r="E12" s="39"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="63">
+        <v>9</v>
+      </c>
       <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D14" s="39"/>
+      <c r="D14" s="63">
+        <v>10</v>
+      </c>
       <c r="E14" s="39"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" s="63">
+        <v>11</v>
+      </c>
       <c r="E15" s="39"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D16" s="39"/>
+      <c r="D16" s="63">
+        <v>12</v>
+      </c>
       <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="63">
+        <v>2</v>
+      </c>
       <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
+      <c r="A18" s="65"/>
       <c r="B18" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C18" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="39"/>
+      <c r="D18" s="63">
+        <v>3</v>
+      </c>
       <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="39"/>
+      <c r="D19" s="63">
+        <v>4</v>
+      </c>
       <c r="E19" s="39"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
+      <c r="A20" s="65"/>
       <c r="B20" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C20" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="39"/>
+      <c r="D20" s="63">
+        <v>7</v>
+      </c>
       <c r="E20" s="39"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C21" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="39"/>
+      <c r="D21" s="63">
+        <v>8</v>
+      </c>
       <c r="E21" s="39"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C22" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="39"/>
+      <c r="D22" s="63">
+        <v>9</v>
+      </c>
       <c r="E22" s="39"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="63">
+        <v>10</v>
+      </c>
       <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="63"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C24" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="39"/>
+      <c r="D24" s="63">
+        <v>11</v>
+      </c>
       <c r="E24" s="39"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C25" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="39"/>
+      <c r="D25" s="63">
+        <v>12</v>
+      </c>
       <c r="E25" s="39"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="63"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C26" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="39"/>
+      <c r="D26" s="63">
+        <v>1</v>
+      </c>
       <c r="E26" s="39"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C27" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="39"/>
+      <c r="D27" s="63">
+        <v>4</v>
+      </c>
       <c r="E27" s="39"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="63"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C28" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="39"/>
+      <c r="D28" s="63">
+        <v>5</v>
+      </c>
       <c r="E28" s="39"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="63"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C29" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="63">
+        <v>10</v>
+      </c>
       <c r="E29" s="39"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="63"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C30" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="39"/>
+      <c r="D30" s="63">
+        <v>11</v>
+      </c>
       <c r="E30" s="39"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="63"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C31" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="39"/>
+      <c r="D31" s="63">
+        <v>1</v>
+      </c>
       <c r="E31" s="39"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="63"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C32" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="39"/>
+      <c r="D32" s="63">
+        <v>2</v>
+      </c>
       <c r="E32" s="39"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="63"/>
+      <c r="A33" s="65"/>
       <c r="B33" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C33" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="39"/>
+      <c r="D33" s="63">
+        <v>3</v>
+      </c>
       <c r="E33" s="39"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="63"/>
+      <c r="A34" s="65"/>
       <c r="B34" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C34" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="63">
+        <v>5</v>
+      </c>
       <c r="E34" s="39"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="63"/>
+      <c r="A35" s="65"/>
       <c r="B35" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C35" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="39"/>
+      <c r="D35" s="63">
+        <v>12</v>
+      </c>
       <c r="E35" s="39"/>
     </row>
     <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="63"/>
+      <c r="A36" s="65"/>
       <c r="B36" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C36" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="63">
+        <v>1</v>
+      </c>
       <c r="E36" s="39"/>
     </row>
     <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="63"/>
+      <c r="A37" s="65"/>
       <c r="B37" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C37" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="39"/>
+      <c r="D37" s="63">
+        <v>2</v>
+      </c>
       <c r="E37" s="39"/>
     </row>
     <row r="38" spans="1:8" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="63"/>
+      <c r="A38" s="65"/>
       <c r="B38" s="56" t="s">
         <v>690</v>
       </c>
       <c r="C38" s="59">
         <v>2011</v>
       </c>
-      <c r="D38" s="56"/>
+      <c r="D38" s="64">
+        <v>1</v>
+      </c>
       <c r="E38" s="56"/>
       <c r="H38" s="58"/>
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="63"/>
+      <c r="A39" s="65"/>
       <c r="B39" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C39" s="42" t="s">
         <v>682</v>
       </c>
-      <c r="D39" s="39"/>
+      <c r="D39" s="63">
+        <v>5</v>
+      </c>
       <c r="E39" s="39"/>
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="63"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C40" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="39"/>
+      <c r="D40" s="63">
+        <v>4</v>
+      </c>
       <c r="E40" s="39"/>
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="63"/>
+      <c r="A41" s="65"/>
       <c r="B41" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C41" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="39"/>
+      <c r="D41" s="63">
+        <v>5</v>
+      </c>
       <c r="E41" s="39"/>
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="63"/>
+      <c r="A42" s="65"/>
       <c r="B42" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C42" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="39"/>
+      <c r="D42" s="63" t="s">
+        <v>692</v>
+      </c>
       <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="63"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C43" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="39"/>
+      <c r="D43" s="63" t="s">
+        <v>693</v>
+      </c>
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="63"/>
+      <c r="A44" s="65"/>
       <c r="B44" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C44" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="39"/>
+      <c r="D44" s="63" t="s">
+        <v>692</v>
+      </c>
       <c r="E44" s="39"/>
     </row>
     <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="63"/>
+      <c r="A45" s="65"/>
       <c r="B45" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C45" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="39"/>
+      <c r="D45" s="63" t="s">
+        <v>694</v>
+      </c>
       <c r="E45" s="39"/>
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="63"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C46" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="39"/>
+      <c r="D46" s="63" t="s">
+        <v>695</v>
+      </c>
       <c r="E46" s="39"/>
     </row>
     <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="63"/>
+      <c r="A47" s="65"/>
       <c r="B47" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C47" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D47" s="39"/>
+      <c r="D47" s="63">
+        <v>2</v>
+      </c>
       <c r="E47" s="39"/>
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="63"/>
+      <c r="A48" s="65"/>
       <c r="B48" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C48" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="39"/>
+      <c r="D48" s="63" t="s">
+        <v>696</v>
+      </c>
       <c r="E48" s="39"/>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="63"/>
+      <c r="A49" s="65"/>
       <c r="B49" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C49" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="39"/>
+      <c r="D49" s="63" t="s">
+        <v>697</v>
+      </c>
       <c r="E49" s="39"/>
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="63"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C50" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="39"/>
+      <c r="D50" s="63" t="s">
+        <v>698</v>
+      </c>
       <c r="E50" s="39"/>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="63"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C51" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="39"/>
+      <c r="D51" s="63" t="s">
+        <v>699</v>
+      </c>
       <c r="E51" s="39"/>
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="63"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C52" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="39"/>
+      <c r="D52" s="63" t="s">
+        <v>692</v>
+      </c>
       <c r="E52" s="39"/>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="63"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C53" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D53" s="39"/>
+      <c r="D53" s="63" t="s">
+        <v>699</v>
+      </c>
       <c r="E53" s="39"/>
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="63"/>
+      <c r="A54" s="65"/>
       <c r="B54" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C54" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="39"/>
+      <c r="D54" s="63" t="s">
+        <v>700</v>
+      </c>
       <c r="E54" s="39"/>
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="63"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C55" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="39"/>
+      <c r="D55" s="63" t="s">
+        <v>696</v>
+      </c>
       <c r="E55" s="39"/>
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="63"/>
+      <c r="A56" s="65"/>
       <c r="B56" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C56" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D56" s="39"/>
+      <c r="D56" s="63" t="s">
+        <v>697</v>
+      </c>
       <c r="E56" s="39"/>
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="63"/>
+      <c r="A57" s="65"/>
       <c r="B57" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C57" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D57" s="39"/>
+      <c r="D57" s="63" t="s">
+        <v>694</v>
+      </c>
       <c r="E57" s="39"/>
     </row>
     <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="63"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C58" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D58" s="39"/>
+      <c r="D58" s="63" t="s">
+        <v>698</v>
+      </c>
       <c r="E58" s="39"/>
     </row>
     <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="63"/>
+      <c r="A59" s="65"/>
       <c r="B59" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C59" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="39"/>
+      <c r="D59" s="63" t="s">
+        <v>695</v>
+      </c>
       <c r="E59" s="39"/>
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="63"/>
+      <c r="A60" s="65"/>
       <c r="B60" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C60" s="42" t="s">
         <v>683</v>
       </c>
-      <c r="D60" s="39"/>
+      <c r="D60" s="63" t="s">
+        <v>701</v>
+      </c>
       <c r="E60" s="39"/>
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="63"/>
+      <c r="A61" s="65"/>
       <c r="B61" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C61" s="42" t="s">
         <v>683</v>
       </c>
-      <c r="D61" s="39"/>
+      <c r="D61" s="63" t="s">
+        <v>700</v>
+      </c>
       <c r="E61" s="39"/>
     </row>
     <row r="62" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="63"/>
+      <c r="A62" s="65"/>
       <c r="B62" s="39" t="s">
         <v>235</v>
       </c>
       <c r="C62" s="42" t="s">
         <v>683</v>
       </c>
-      <c r="D62" s="39"/>
+      <c r="D62" s="63" t="s">
+        <v>697</v>
+      </c>
       <c r="E62" s="39"/>
     </row>
     <row r="63" spans="1:8" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="63"/>
+      <c r="A63" s="65"/>
       <c r="B63" s="56" t="s">
         <v>688</v>
       </c>
       <c r="C63" s="59"/>
-      <c r="D63" s="56"/>
+      <c r="D63" s="64"/>
       <c r="E63" s="56"/>
       <c r="H63" s="58"/>
     </row>
     <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="63"/>
+      <c r="A64" s="65"/>
       <c r="B64" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C64" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D64" s="39"/>
+      <c r="D64" s="63" t="s">
+        <v>701</v>
+      </c>
       <c r="E64" s="39"/>
     </row>
     <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="63"/>
+      <c r="A65" s="65"/>
       <c r="B65" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C65" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D65" s="39"/>
+      <c r="D65" s="63" t="s">
+        <v>699</v>
+      </c>
       <c r="E65" s="39"/>
     </row>
     <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="63"/>
+      <c r="A66" s="65"/>
       <c r="B66" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C66" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D66" s="39"/>
+      <c r="D66" s="63" t="s">
+        <v>700</v>
+      </c>
       <c r="E66" s="39"/>
     </row>
     <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="63"/>
+      <c r="A67" s="65"/>
       <c r="B67" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C67" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D67" s="39"/>
+      <c r="D67" s="63" t="s">
+        <v>702</v>
+      </c>
       <c r="E67" s="39"/>
     </row>
     <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="63"/>
+      <c r="A68" s="65"/>
       <c r="B68" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C68" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D68" s="39"/>
+      <c r="D68" s="63" t="s">
+        <v>701</v>
+      </c>
       <c r="E68" s="39"/>
     </row>
     <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A69" s="63"/>
+      <c r="A69" s="65"/>
       <c r="B69" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C69" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D69" s="39"/>
+      <c r="D69" s="63" t="s">
+        <v>699</v>
+      </c>
       <c r="E69" s="39"/>
     </row>
     <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A70" s="63"/>
+      <c r="A70" s="65"/>
       <c r="B70" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C70" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D70" s="39"/>
+      <c r="D70" s="63" t="s">
+        <v>700</v>
+      </c>
       <c r="E70" s="39"/>
     </row>
     <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="63"/>
+      <c r="A71" s="65"/>
       <c r="B71" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C71" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D71" s="39"/>
+      <c r="D71" s="63" t="s">
+        <v>693</v>
+      </c>
       <c r="E71" s="39"/>
     </row>
     <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A72" s="63"/>
+      <c r="A72" s="65"/>
       <c r="B72" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C72" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D72" s="39"/>
+      <c r="D72" s="63" t="s">
+        <v>696</v>
+      </c>
       <c r="E72" s="39"/>
     </row>
     <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="63"/>
+      <c r="A73" s="65"/>
       <c r="B73" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C73" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D73" s="39"/>
+      <c r="D73" s="63" t="s">
+        <v>702</v>
+      </c>
       <c r="E73" s="39"/>
     </row>
     <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="63"/>
+      <c r="A74" s="65"/>
       <c r="B74" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C74" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D74" s="39"/>
+      <c r="D74" s="63" t="s">
+        <v>701</v>
+      </c>
       <c r="E74" s="39"/>
     </row>
     <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A75" s="63"/>
+      <c r="A75" s="65"/>
       <c r="B75" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C75" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D75" s="39"/>
+      <c r="D75" s="63" t="s">
+        <v>699</v>
+      </c>
       <c r="E75" s="39"/>
     </row>
     <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="63"/>
+      <c r="A76" s="65"/>
       <c r="B76" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C76" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D76" s="39"/>
+      <c r="D76" s="63" t="s">
+        <v>700</v>
+      </c>
       <c r="E76" s="39"/>
     </row>
     <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="63"/>
+      <c r="A77" s="65"/>
       <c r="B77" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C77" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D77" s="39"/>
+      <c r="D77" s="63" t="s">
+        <v>693</v>
+      </c>
       <c r="E77" s="39"/>
     </row>
     <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="63"/>
+      <c r="A78" s="65"/>
       <c r="B78" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C78" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D78" s="39"/>
+      <c r="D78" s="63" t="s">
+        <v>700</v>
+      </c>
       <c r="E78" s="39"/>
     </row>
     <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="63"/>
+      <c r="A79" s="65"/>
       <c r="B79" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C79" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D79" s="39"/>
+      <c r="D79" s="63" t="s">
+        <v>693</v>
+      </c>
       <c r="E79" s="39"/>
     </row>
     <row r="80" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A80" s="63"/>
+      <c r="A80" s="65"/>
       <c r="B80" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C80" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D80" s="39"/>
+      <c r="D80" s="63" t="s">
+        <v>696</v>
+      </c>
       <c r="E80" s="39"/>
     </row>
     <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="63"/>
+      <c r="A81" s="65"/>
       <c r="B81" s="39" t="s">
         <v>332</v>
       </c>
       <c r="C81" s="42" t="s">
         <v>683</v>
       </c>
-      <c r="D81" s="39"/>
+      <c r="D81" s="63" t="s">
+        <v>702</v>
+      </c>
       <c r="E81" s="39"/>
     </row>
     <row r="82" spans="1:8" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="64"/>
+      <c r="A82" s="66"/>
       <c r="B82" s="56" t="s">
         <v>361</v>
       </c>
       <c r="C82" s="59">
         <v>2015</v>
       </c>
-      <c r="D82" s="56"/>
+      <c r="D82" s="64" t="s">
+        <v>702</v>
+      </c>
       <c r="E82" s="56"/>
       <c r="H82" s="58"/>
     </row>
     <row r="83" spans="1:8" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A83" s="64"/>
+      <c r="A83" s="66"/>
       <c r="B83" s="56" t="s">
         <v>361</v>
       </c>
       <c r="C83" s="59">
         <v>2015</v>
       </c>
-      <c r="D83" s="56"/>
+      <c r="D83" s="64" t="s">
+        <v>701</v>
+      </c>
       <c r="E83" s="56"/>
       <c r="H83" s="58"/>
     </row>
     <row r="84" spans="1:8" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A84" s="64"/>
+      <c r="A84" s="66"/>
       <c r="B84" s="56" t="s">
         <v>361</v>
       </c>
       <c r="C84" s="59">
         <v>2016</v>
       </c>
-      <c r="D84" s="56"/>
+      <c r="D84" s="64" t="s">
+        <v>703</v>
+      </c>
       <c r="E84" s="56"/>
       <c r="H84" s="58"/>
     </row>
     <row r="85" spans="1:8" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A85" s="64"/>
+      <c r="A85" s="66"/>
       <c r="B85" s="56" t="s">
         <v>361</v>
       </c>
       <c r="C85" s="59">
         <v>2016</v>
       </c>
-      <c r="D85" s="56"/>
+      <c r="D85" s="64" t="s">
+        <v>704</v>
+      </c>
       <c r="E85" s="56"/>
       <c r="H85" s="58"/>
     </row>
     <row r="86" spans="1:8" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A86" s="64"/>
+      <c r="A86" s="66"/>
       <c r="B86" s="56" t="s">
         <v>361</v>
       </c>
       <c r="C86" s="59">
         <v>2016</v>
       </c>
-      <c r="D86" s="56"/>
+      <c r="D86" s="64" t="s">
+        <v>697</v>
+      </c>
       <c r="E86" s="56"/>
       <c r="H86" s="58"/>
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="63"/>
+      <c r="A87" s="65"/>
       <c r="B87" s="39" t="s">
         <v>375</v>
       </c>
       <c r="C87" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D87" s="39"/>
+      <c r="D87" s="63" t="s">
+        <v>696</v>
+      </c>
       <c r="E87" s="39"/>
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="63"/>
+      <c r="A88" s="65"/>
       <c r="B88" s="39" t="s">
         <v>375</v>
       </c>
       <c r="C88" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D88" s="39"/>
+      <c r="D88" s="63" t="s">
+        <v>703</v>
+      </c>
       <c r="E88" s="39"/>
     </row>
     <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="63"/>
+      <c r="A89" s="65"/>
       <c r="B89" s="39" t="s">
         <v>375</v>
       </c>
       <c r="C89" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D89" s="39"/>
+      <c r="D89" s="63" t="s">
+        <v>704</v>
+      </c>
       <c r="E89" s="39"/>
     </row>
     <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A90" s="63"/>
+      <c r="A90" s="65"/>
       <c r="B90" s="39" t="s">
         <v>375</v>
       </c>
       <c r="C90" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D90" s="39"/>
+      <c r="D90" s="63" t="s">
+        <v>697</v>
+      </c>
       <c r="E90" s="39"/>
     </row>
     <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A91" s="63"/>
+      <c r="A91" s="65"/>
       <c r="B91" s="39" t="s">
         <v>393</v>
       </c>
       <c r="C91" s="42">
         <v>2015</v>
       </c>
-      <c r="D91" s="39"/>
+      <c r="D91" s="63" t="s">
+        <v>694</v>
+      </c>
       <c r="E91" s="39"/>
     </row>
     <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A92" s="63"/>
+      <c r="A92" s="65"/>
       <c r="B92" s="39" t="s">
         <v>393</v>
       </c>
       <c r="C92" s="42">
         <v>2015</v>
       </c>
-      <c r="D92" s="39"/>
+      <c r="D92" s="63" t="s">
+        <v>698</v>
+      </c>
       <c r="E92" s="39"/>
     </row>
     <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A93" s="63"/>
+      <c r="A93" s="65"/>
       <c r="B93" s="39" t="s">
         <v>393</v>
       </c>
       <c r="C93" s="42">
         <v>2015</v>
       </c>
-      <c r="D93" s="39"/>
+      <c r="D93" s="63" t="s">
+        <v>705</v>
+      </c>
       <c r="E93" s="39"/>
     </row>
     <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A94" s="63"/>
+      <c r="A94" s="65"/>
       <c r="B94" s="39" t="s">
         <v>393</v>
       </c>
       <c r="C94" s="42">
         <v>2016</v>
       </c>
-      <c r="D94" s="39"/>
+      <c r="D94" s="63" t="s">
+        <v>701</v>
+      </c>
       <c r="E94" s="39"/>
     </row>
     <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -25621,7 +25885,9 @@
       <c r="C95" s="42">
         <v>2016</v>
       </c>
-      <c r="D95" s="39"/>
+      <c r="D95" s="63" t="s">
+        <v>699</v>
+      </c>
       <c r="E95" s="39"/>
     </row>
     <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -25632,7 +25898,9 @@
       <c r="C96" s="42">
         <v>2016</v>
       </c>
-      <c r="D96" s="39"/>
+      <c r="D96" s="63" t="s">
+        <v>693</v>
+      </c>
       <c r="E96" s="39"/>
     </row>
     <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25643,7 +25911,9 @@
       <c r="C97" s="42">
         <v>2016</v>
       </c>
-      <c r="D97" s="39"/>
+      <c r="D97" s="63" t="s">
+        <v>697</v>
+      </c>
       <c r="E97" s="39"/>
     </row>
     <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25654,7 +25924,9 @@
       <c r="C98" s="42">
         <v>2016</v>
       </c>
-      <c r="D98" s="39"/>
+      <c r="D98" s="63" t="s">
+        <v>694</v>
+      </c>
       <c r="E98" s="39"/>
     </row>
     <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25665,7 +25937,9 @@
       <c r="C99" s="42">
         <v>2016</v>
       </c>
-      <c r="D99" s="39"/>
+      <c r="D99" s="63" t="s">
+        <v>698</v>
+      </c>
       <c r="E99" s="39"/>
     </row>
     <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25676,7 +25950,9 @@
       <c r="C100" s="42">
         <v>2017</v>
       </c>
-      <c r="D100" s="39"/>
+      <c r="D100" s="63" t="s">
+        <v>702</v>
+      </c>
       <c r="E100" s="39"/>
     </row>
     <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25687,7 +25963,9 @@
       <c r="C101" s="42">
         <v>2017</v>
       </c>
-      <c r="D101" s="39"/>
+      <c r="D101" s="63" t="s">
+        <v>701</v>
+      </c>
       <c r="E101" s="39"/>
     </row>
     <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25698,7 +25976,9 @@
       <c r="C102" s="42">
         <v>2017</v>
       </c>
-      <c r="D102" s="39"/>
+      <c r="D102" s="63" t="s">
+        <v>699</v>
+      </c>
       <c r="E102" s="39"/>
     </row>
     <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25709,7 +25989,9 @@
       <c r="C103" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D103" s="39"/>
+      <c r="D103" s="63" t="s">
+        <v>693</v>
+      </c>
       <c r="E103" s="39"/>
     </row>
     <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25720,7 +26002,9 @@
       <c r="C104" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D104" s="39"/>
+      <c r="D104" s="63" t="s">
+        <v>700</v>
+      </c>
       <c r="E104" s="39"/>
     </row>
     <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25731,7 +26015,9 @@
       <c r="C105" s="42">
         <v>2013</v>
       </c>
-      <c r="D105" s="39"/>
+      <c r="D105" s="63" t="s">
+        <v>706</v>
+      </c>
       <c r="E105" s="39"/>
     </row>
     <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25742,7 +26028,9 @@
       <c r="C106" s="42">
         <v>2014</v>
       </c>
-      <c r="D106" s="39"/>
+      <c r="D106" s="63" t="s">
+        <v>707</v>
+      </c>
       <c r="E106" s="39"/>
     </row>
     <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25753,7 +26041,9 @@
       <c r="C107" s="42">
         <v>2014</v>
       </c>
-      <c r="D107" s="39"/>
+      <c r="D107" s="63" t="s">
+        <v>708</v>
+      </c>
       <c r="E107" s="39"/>
     </row>
     <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25764,7 +26054,9 @@
       <c r="C108" s="42">
         <v>2015</v>
       </c>
-      <c r="D108" s="39"/>
+      <c r="D108" s="63" t="s">
+        <v>709</v>
+      </c>
       <c r="E108" s="39"/>
     </row>
     <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25775,7 +26067,9 @@
       <c r="C109" s="42">
         <v>2016</v>
       </c>
-      <c r="D109" s="39"/>
+      <c r="D109" s="63" t="s">
+        <v>710</v>
+      </c>
       <c r="E109" s="39"/>
     </row>
     <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -25784,7 +26078,9 @@
         <v>436</v>
       </c>
       <c r="C110" s="62"/>
-      <c r="D110" s="39"/>
+      <c r="D110" s="63" t="s">
+        <v>711</v>
+      </c>
       <c r="E110" s="39"/>
       <c r="F110" s="57"/>
     </row>
@@ -25794,7 +26090,9 @@
         <v>436</v>
       </c>
       <c r="C111" s="62"/>
-      <c r="D111" s="39"/>
+      <c r="D111" s="63" t="s">
+        <v>712</v>
+      </c>
       <c r="E111" s="39"/>
       <c r="F111" s="57"/>
     </row>
@@ -25806,7 +26104,9 @@
       <c r="C112" s="42">
         <v>2010</v>
       </c>
-      <c r="D112" s="39"/>
+      <c r="D112" s="63" t="s">
+        <v>713</v>
+      </c>
       <c r="E112" s="39"/>
       <c r="F112" s="43"/>
     </row>
@@ -25818,7 +26118,9 @@
       <c r="C113" s="42">
         <v>2010</v>
       </c>
-      <c r="D113" s="39"/>
+      <c r="D113" s="63" t="s">
+        <v>714</v>
+      </c>
       <c r="E113" s="39"/>
     </row>
     <row r="114" spans="1:8" s="57" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -25829,7 +26131,9 @@
       <c r="C114" s="59">
         <v>2016</v>
       </c>
-      <c r="D114" s="56"/>
+      <c r="D114" s="64" t="s">
+        <v>703</v>
+      </c>
       <c r="E114" s="56"/>
       <c r="H114" s="58"/>
     </row>
@@ -25841,7 +26145,7 @@
       <c r="C115" s="59">
         <v>2016</v>
       </c>
-      <c r="D115" s="56"/>
+      <c r="D115" s="64"/>
       <c r="E115" s="56"/>
       <c r="H115" s="58"/>
     </row>
@@ -25853,7 +26157,9 @@
       <c r="C116" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D116" s="39"/>
+      <c r="D116" s="63" t="s">
+        <v>702</v>
+      </c>
       <c r="E116" s="39"/>
     </row>
     <row r="117" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -25864,7 +26170,9 @@
       <c r="C117" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D117" s="39"/>
+      <c r="D117" s="63" t="s">
+        <v>702</v>
+      </c>
       <c r="E117" s="39"/>
     </row>
     <row r="118" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>